<commit_message>
Irfan - Updates to testdata
</commit_message>
<xml_diff>
--- a/goldendata/Assignment2Part1NoRDO/Part1_RDO_Disabled_Testdata.xlsx
+++ b/goldendata/Assignment2Part1NoRDO/Part1_RDO_Disabled_Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="31">
   <si>
     <t>Block = 8</t>
   </si>
@@ -104,12 +104,18 @@
   <si>
     <t>Execution Time</t>
   </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,16 +131,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -142,19 +160,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -204,7 +287,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>RD plot i=16,</a:t>
+              <a:t>Rate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Distortion P</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>lot i=16,</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -487,11 +578,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="391277632"/>
-        <c:axId val="391279592"/>
+        <c:axId val="490776960"/>
+        <c:axId val="490780488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="391277632"/>
+        <c:axId val="490776960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,12 +695,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391279592"/>
+        <c:crossAx val="490780488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="391279592"/>
+        <c:axId val="490780488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391277632"/>
+        <c:crossAx val="490776960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -838,11 +929,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>RD plot</a:t>
+              <a:t>Rate</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> i=8, r=2 RDO Disabled</a:t>
+              <a:t> Distortion P</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>lot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> i=8, r=2, RDO Disabled</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1114,11 +1213,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="391281552"/>
-        <c:axId val="392653792"/>
+        <c:axId val="490784408"/>
+        <c:axId val="490785976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="391281552"/>
+        <c:axId val="490784408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,12 +1330,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392653792"/>
+        <c:crossAx val="490785976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="392653792"/>
+        <c:axId val="490785976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391281552"/>
+        <c:crossAx val="490784408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1627,11 +1726,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="392655360"/>
-        <c:axId val="392654184"/>
+        <c:axId val="490784016"/>
+        <c:axId val="490785192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="392655360"/>
+        <c:axId val="490784016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,12 +1848,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392654184"/>
+        <c:crossAx val="490785192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="392654184"/>
+        <c:axId val="490785192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1966,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392655360"/>
+        <c:crossAx val="490784016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4000,8 +4099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4031,22 +4130,22 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4155,22 +4254,22 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4268,42 +4367,44 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4334,28 +4435,29 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4386,28 +4488,29 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F24" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4437,6 +4540,25 @@
         <v>101.51</v>
       </c>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
@@ -4454,7 +4576,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="A19:D19"/>
     <mergeCell ref="A18:I18"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:D10"/>
@@ -4474,7 +4598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>

</xml_diff>